<commit_message>
Refactored test to submit more than 1 experiment
</commit_message>
<xml_diff>
--- a/frontend/cypress/fixtures/Experiment_submission_v3_3_0_F_A_1.xlsx
+++ b/frontend/cypress/fixtures/Experiment_submission_v3_3_0_F_A_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/frontend/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FCE577-7EC1-E148-87FA-29F0A8EBCE88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935B8FF1-77B0-B045-B686-D4DB58CCCB59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="22540" xr2:uid="{081C58B0-D29E-7C46-A768-7ECA00AF7D31}"/>
   </bookViews>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="109">
   <si>
     <t>Experiment Submission Template</t>
   </si>
@@ -479,13 +479,16 @@
     <t>scanchiprackbarcodehere</t>
   </si>
   <si>
-    <t>CONTAINERFOREXPMULTIPLE</t>
-  </si>
-  <si>
     <t>THEBARCODE</t>
   </si>
   <si>
     <t>YD-1417</t>
+  </si>
+  <si>
+    <t>CONTAINERFOREXPMULTIPLE7</t>
+  </si>
+  <si>
+    <t>CONTAINERFOREXPMULTIPLE8</t>
   </si>
 </sst>
 </file>
@@ -1161,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F052AE-ADF9-394E-B4E9-F15CBD15E504}">
   <dimension ref="A1:AP215"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1539,10 +1542,10 @@
         <v>1</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D12" t="s">
         <v>58</v>
@@ -1554,7 +1557,7 @@
         <v>44377</v>
       </c>
       <c r="G12" s="43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H12" s="2">
         <v>44312</v>
@@ -1650,17 +1653,121 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:42" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="23">
         <v>2</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="2"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="42"/>
-      <c r="X13" s="41"/>
-      <c r="Y13" s="41"/>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="2">
+        <v>44377</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" s="2">
+        <v>44312</v>
+      </c>
+      <c r="I13" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13" t="s">
+        <v>82</v>
+      </c>
+      <c r="K13" t="s">
+        <v>83</v>
+      </c>
+      <c r="L13" s="41">
+        <v>0.125</v>
+      </c>
+      <c r="M13" s="42">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="N13" t="s">
+        <v>84</v>
+      </c>
+      <c r="O13" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>86</v>
+      </c>
+      <c r="R13" t="s">
+        <v>87</v>
+      </c>
+      <c r="S13" t="s">
+        <v>88</v>
+      </c>
+      <c r="T13" t="s">
+        <v>89</v>
+      </c>
+      <c r="U13" t="s">
+        <v>90</v>
+      </c>
+      <c r="V13" t="s">
+        <v>91</v>
+      </c>
+      <c r="W13" t="s">
+        <v>92</v>
+      </c>
+      <c r="X13" s="41">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="Y13" s="41">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>98</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>102</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>103</v>
+      </c>
+      <c r="AO13" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A14" s="23">
@@ -2687,10 +2794,10 @@
         <v>101</v>
       </c>
       <c r="B117">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C117" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E117">
         <v>5</v>

</xml_diff>

<commit_message>
Created more exhaustive tests and incorporated a more complete template
</commit_message>
<xml_diff>
--- a/frontend/cypress/fixtures/Experiment_submission_v3_3_0_F_A_1.xlsx
+++ b/frontend/cypress/fixtures/Experiment_submission_v3_3_0_F_A_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/frontend/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935B8FF1-77B0-B045-B686-D4DB58CCCB59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C704C412-9819-9440-BE53-6DE247C9DA69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="22540" xr2:uid="{081C58B0-D29E-7C46-A768-7ECA00AF7D31}"/>
   </bookViews>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="110">
   <si>
     <t>Experiment Submission Template</t>
   </si>
@@ -338,9 +338,6 @@
     <t>Comment Scan</t>
   </si>
   <si>
-    <t>infinium gs 24 beadchip</t>
-  </si>
-  <si>
     <t>iScan_1</t>
   </si>
   <si>
@@ -482,13 +479,19 @@
     <t>THEBARCODE</t>
   </si>
   <si>
-    <t>YD-1417</t>
-  </si>
-  <si>
-    <t>CONTAINERFOREXPMULTIPLE7</t>
-  </si>
-  <si>
-    <t>CONTAINERFOREXPMULTIPLE8</t>
+    <t>test_abc1</t>
+  </si>
+  <si>
+    <t>96-well plate</t>
+  </si>
+  <si>
+    <t>test_qwe2</t>
+  </si>
+  <si>
+    <t>B02</t>
+  </si>
+  <si>
+    <t>B03</t>
   </si>
 </sst>
 </file>
@@ -1164,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F052AE-ADF9-394E-B4E9-F15CBD15E504}">
   <dimension ref="A1:AP215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1545,31 +1548,31 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" t="s">
         <v>58</v>
-      </c>
-      <c r="E12" t="s">
-        <v>59</v>
       </c>
       <c r="F12" s="2">
         <v>44377</v>
       </c>
       <c r="G12" s="43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H12" s="2">
         <v>44312</v>
       </c>
       <c r="I12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" t="s">
         <v>81</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>82</v>
-      </c>
-      <c r="K12" t="s">
-        <v>83</v>
       </c>
       <c r="L12" s="41">
         <v>0.125</v>
@@ -1578,31 +1581,31 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="N12" t="s">
+        <v>83</v>
+      </c>
+      <c r="O12" t="s">
         <v>84</v>
       </c>
-      <c r="O12" t="s">
+      <c r="Q12" t="s">
         <v>85</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>86</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>87</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>88</v>
       </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
         <v>89</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>90</v>
       </c>
-      <c r="V12" t="s">
+      <c r="W12" t="s">
         <v>91</v>
-      </c>
-      <c r="W12" t="s">
-        <v>92</v>
       </c>
       <c r="X12" s="41">
         <v>8.3333333333333329E-2</v>
@@ -1611,46 +1614,46 @@
         <v>0.10416666666666667</v>
       </c>
       <c r="AA12" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC12" t="s">
         <v>93</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AD12" t="s">
         <v>94</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>95</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AF12" t="s">
         <v>96</v>
       </c>
-      <c r="AF12" t="s">
+      <c r="AG12" t="s">
         <v>97</v>
       </c>
-      <c r="AG12" t="s">
+      <c r="AH12" t="s">
         <v>98</v>
       </c>
-      <c r="AH12" t="s">
+      <c r="AI12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ12" t="s">
         <v>99</v>
       </c>
-      <c r="AI12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ12" t="s">
+      <c r="AK12" t="s">
         <v>100</v>
       </c>
-      <c r="AK12" t="s">
+      <c r="AL12" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM12" t="s">
         <v>101</v>
       </c>
-      <c r="AL12" t="s">
-        <v>92</v>
-      </c>
-      <c r="AM12" t="s">
+      <c r="AN12" t="s">
         <v>102</v>
       </c>
-      <c r="AN12" t="s">
+      <c r="AO12" t="s">
         <v>103</v>
-      </c>
-      <c r="AO12" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:42" ht="17" x14ac:dyDescent="0.2">
@@ -1661,31 +1664,31 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" t="s">
         <v>58</v>
-      </c>
-      <c r="E13" t="s">
-        <v>59</v>
       </c>
       <c r="F13" s="2">
         <v>44377</v>
       </c>
       <c r="G13" s="43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H13" s="2">
         <v>44312</v>
       </c>
       <c r="I13" t="s">
+        <v>80</v>
+      </c>
+      <c r="J13" t="s">
         <v>81</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>82</v>
-      </c>
-      <c r="K13" t="s">
-        <v>83</v>
       </c>
       <c r="L13" s="41">
         <v>0.125</v>
@@ -1694,31 +1697,31 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="N13" t="s">
+        <v>83</v>
+      </c>
+      <c r="O13" t="s">
         <v>84</v>
       </c>
-      <c r="O13" t="s">
+      <c r="Q13" t="s">
         <v>85</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>86</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>87</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>88</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>89</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
         <v>90</v>
       </c>
-      <c r="V13" t="s">
+      <c r="W13" t="s">
         <v>91</v>
-      </c>
-      <c r="W13" t="s">
-        <v>92</v>
       </c>
       <c r="X13" s="41">
         <v>8.3333333333333329E-2</v>
@@ -1727,46 +1730,46 @@
         <v>0.10416666666666667</v>
       </c>
       <c r="AA13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC13" t="s">
         <v>93</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AD13" t="s">
         <v>94</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AE13" t="s">
         <v>95</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AF13" t="s">
         <v>96</v>
       </c>
-      <c r="AF13" t="s">
+      <c r="AG13" t="s">
         <v>97</v>
       </c>
-      <c r="AG13" t="s">
+      <c r="AH13" t="s">
         <v>98</v>
       </c>
-      <c r="AH13" t="s">
+      <c r="AI13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ13" t="s">
         <v>99</v>
       </c>
-      <c r="AI13" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ13" t="s">
+      <c r="AK13" t="s">
         <v>100</v>
       </c>
-      <c r="AK13" t="s">
+      <c r="AL13" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM13" t="s">
         <v>101</v>
       </c>
-      <c r="AL13" t="s">
-        <v>92</v>
-      </c>
-      <c r="AM13" t="s">
+      <c r="AN13" t="s">
         <v>102</v>
       </c>
-      <c r="AN13" t="s">
+      <c r="AO13" t="s">
         <v>103</v>
-      </c>
-      <c r="AO13" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.2">
@@ -2762,7 +2765,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B115" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C115" s="25"/>
       <c r="D115" s="25"/>
@@ -2777,16 +2780,16 @@
         <v>17</v>
       </c>
       <c r="C116" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D116" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D116" s="27" t="s">
+      <c r="E116" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="E116" s="27" t="s">
+      <c r="F116" s="27" t="s">
         <v>63</v>
-      </c>
-      <c r="F116" s="27" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -2797,18 +2800,36 @@
         <v>7</v>
       </c>
       <c r="C117" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="D117" t="s">
+        <v>64</v>
       </c>
       <c r="E117">
         <v>5</v>
       </c>
       <c r="F117" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="23">
         <v>102</v>
+      </c>
+      <c r="B118">
+        <v>8</v>
+      </c>
+      <c r="C118" t="s">
+        <v>107</v>
+      </c>
+      <c r="D118" t="s">
+        <v>64</v>
+      </c>
+      <c r="E118">
+        <v>3</v>
+      </c>
+      <c r="F118" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -3319,27 +3340,27 @@
         <v>9</v>
       </c>
       <c r="B1" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
         <v>66</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="E1" t="s">
         <v>68</v>
-      </c>
-      <c r="E1" t="s">
-        <v>69</v>
       </c>
       <c r="F1" t="s">
         <v>14</v>
       </c>
       <c r="G1" s="40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
@@ -3348,16 +3369,16 @@
         <v>32</v>
       </c>
       <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
         <v>72</v>
-      </c>
-      <c r="E2" t="s">
-        <v>73</v>
       </c>
       <c r="F2" t="s">
         <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -3365,22 +3386,22 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
         <v>75</v>
-      </c>
-      <c r="C3" t="s">
-        <v>76</v>
       </c>
       <c r="D3" t="s">
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F3" t="s">
         <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -3388,7 +3409,7 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
         <v>37</v>
@@ -3397,7 +3418,7 @@
         <v>46</v>
       </c>
       <c r="G4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3405,7 +3426,7 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
         <v>47</v>
@@ -3416,7 +3437,7 @@
         <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
         <v>48</v>
@@ -3424,29 +3445,29 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
         <v>79</v>
       </c>
-      <c r="D7" t="s">
-        <v>80</v>
-      </c>
       <c r="F7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" t="s">
         <v>75</v>
-      </c>
-      <c r="F8" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F9" t="s">
         <v>51</v>
@@ -3459,12 +3480,12 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>